<commit_message>
Creating new day averages
</commit_message>
<xml_diff>
--- a/Data/Dailies.xlsx
+++ b/Data/Dailies.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryan\Coding Projects\Dalies\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7238082C-F265-44C6-AA69-7BEFEB125630}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{287DAA61-79A3-4439-96CC-58D94B44687B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{5AECCF6F-801D-49D3-972A-947870F3C920}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1671" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1718" uniqueCount="18">
   <si>
     <t xml:space="preserve">Date </t>
   </si>
@@ -89,21 +89,6 @@
   </si>
   <si>
     <t>Language</t>
-  </si>
-  <si>
-    <t>Column28</t>
-  </si>
-  <si>
-    <t>Sum</t>
-  </si>
-  <si>
-    <t>Average</t>
-  </si>
-  <si>
-    <t>Running Total</t>
-  </si>
-  <si>
-    <t>Count</t>
   </si>
 </sst>
 </file>
@@ -456,11 +441,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4D90D68-022F-4D80-B45F-E8F95C295EA5}">
-  <dimension ref="A1:O290"/>
+  <dimension ref="A1:O297"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A266" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P283" sqref="P283"/>
+      <selection pane="bottomLeft" activeCell="N293" sqref="N293"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6915,6 +6900,197 @@
         <v>1</v>
       </c>
     </row>
+    <row r="291" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A291" s="1">
+        <v>45096</v>
+      </c>
+      <c r="B291" t="s">
+        <v>12</v>
+      </c>
+      <c r="C291" t="s">
+        <v>1</v>
+      </c>
+      <c r="D291" t="s">
+        <v>1</v>
+      </c>
+      <c r="F291" t="s">
+        <v>1</v>
+      </c>
+      <c r="G291" t="s">
+        <v>1</v>
+      </c>
+      <c r="H291" t="s">
+        <v>13</v>
+      </c>
+      <c r="L291" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="292" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A292" s="1">
+        <v>45097</v>
+      </c>
+      <c r="B292" t="s">
+        <v>12</v>
+      </c>
+      <c r="D292" t="s">
+        <v>1</v>
+      </c>
+      <c r="E292" t="s">
+        <v>1</v>
+      </c>
+      <c r="F292" t="s">
+        <v>1</v>
+      </c>
+      <c r="G292" t="s">
+        <v>1</v>
+      </c>
+      <c r="H292" t="s">
+        <v>13</v>
+      </c>
+      <c r="K292" t="s">
+        <v>1</v>
+      </c>
+      <c r="N292" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="293" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A293" s="1">
+        <v>45098</v>
+      </c>
+      <c r="B293" t="s">
+        <v>12</v>
+      </c>
+      <c r="C293" t="s">
+        <v>1</v>
+      </c>
+      <c r="D293" t="s">
+        <v>1</v>
+      </c>
+      <c r="E293" t="s">
+        <v>1</v>
+      </c>
+      <c r="F293" t="s">
+        <v>1</v>
+      </c>
+      <c r="G293" t="s">
+        <v>1</v>
+      </c>
+      <c r="H293" t="s">
+        <v>13</v>
+      </c>
+      <c r="I293" t="s">
+        <v>1</v>
+      </c>
+      <c r="L293" t="s">
+        <v>1</v>
+      </c>
+      <c r="N293" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="294" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A294" s="1">
+        <v>45099</v>
+      </c>
+      <c r="B294" t="s">
+        <v>12</v>
+      </c>
+      <c r="D294" t="s">
+        <v>1</v>
+      </c>
+      <c r="F294" t="s">
+        <v>1</v>
+      </c>
+      <c r="G294" t="s">
+        <v>1</v>
+      </c>
+      <c r="H294" t="s">
+        <v>13</v>
+      </c>
+      <c r="N294" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="295" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A295" s="1">
+        <v>45100</v>
+      </c>
+      <c r="B295" t="s">
+        <v>12</v>
+      </c>
+      <c r="F295" t="s">
+        <v>1</v>
+      </c>
+      <c r="G295" t="s">
+        <v>1</v>
+      </c>
+      <c r="H295" t="s">
+        <v>13</v>
+      </c>
+      <c r="L295" t="s">
+        <v>1</v>
+      </c>
+      <c r="N295" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="296" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A296" s="1">
+        <v>45101</v>
+      </c>
+      <c r="B296" t="s">
+        <v>12</v>
+      </c>
+      <c r="C296" t="s">
+        <v>1</v>
+      </c>
+      <c r="F296" t="s">
+        <v>1</v>
+      </c>
+      <c r="G296" t="s">
+        <v>1</v>
+      </c>
+      <c r="I296" t="s">
+        <v>1</v>
+      </c>
+      <c r="L296" t="s">
+        <v>1</v>
+      </c>
+      <c r="N296" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="297" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A297" s="1">
+        <v>45102</v>
+      </c>
+      <c r="B297" t="s">
+        <v>12</v>
+      </c>
+      <c r="D297" t="s">
+        <v>1</v>
+      </c>
+      <c r="E297" t="s">
+        <v>1</v>
+      </c>
+      <c r="G297" t="s">
+        <v>1</v>
+      </c>
+      <c r="H297" t="s">
+        <v>13</v>
+      </c>
+      <c r="K297" t="s">
+        <v>1</v>
+      </c>
+      <c r="L297" t="s">
+        <v>1</v>
+      </c>
+      <c r="N297" t="s">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>